<commit_message>
added leave days & adjust col width
</commit_message>
<xml_diff>
--- a/public/timesheet_template.xlsx
+++ b/public/timesheet_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevEnv\workspace\pj\timesheet-creator\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F323955-3190-4649-89EF-0906F23168C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCCDD93-4EFF-41BD-9C88-CE81AB481602}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Automated Form - ONLY Modify D9" sheetId="1" r:id="rId1"/>
@@ -727,6 +727,138 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="179" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -736,255 +868,123 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1565,7 +1565,7 @@
   </sheetPr>
   <dimension ref="A1:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
@@ -1590,259 +1590,259 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="112" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
+      <c r="B1" s="112"/>
+      <c r="C1" s="112"/>
+      <c r="D1" s="112"/>
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
     </row>
     <row r="2" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="134" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
+      <c r="B2" s="134"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="134"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134"/>
+      <c r="O2" s="134"/>
     </row>
     <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="55"/>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="56"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="101"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="101"/>
+      <c r="H4" s="101"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="101"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="101"/>
+      <c r="M4" s="101"/>
+      <c r="N4" s="101"/>
+      <c r="O4" s="102"/>
     </row>
     <row r="5" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="130" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="58" t="s">
+      <c r="B5" s="130"/>
+      <c r="C5" s="130"/>
+      <c r="D5" s="135" t="s">
         <v>63</v>
       </c>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
+      <c r="N5" s="135"/>
+      <c r="O5" s="135"/>
     </row>
     <row r="6" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="49" t="s">
+      <c r="B6" s="94"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="50"/>
-      <c r="M6" s="50"/>
-      <c r="N6" s="50"/>
-      <c r="O6" s="51"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="94"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="94"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="95"/>
     </row>
     <row r="7" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="A7" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="50" t="s">
+      <c r="B7" s="94"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="50"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="50"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="50"/>
-      <c r="O7" s="51"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="94"/>
+      <c r="L7" s="94"/>
+      <c r="M7" s="94"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="95"/>
     </row>
     <row r="8" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59" t="s">
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59" t="s">
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="131" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59" t="s">
+      <c r="I8" s="131"/>
+      <c r="J8" s="131"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="131" t="s">
         <v>30</v>
       </c>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
+      <c r="M8" s="131"/>
+      <c r="N8" s="131"/>
+      <c r="O8" s="131"/>
     </row>
     <row r="9" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="60">
+      <c r="B9" s="130"/>
+      <c r="C9" s="130"/>
+      <c r="D9" s="132">
         <v>45078</v>
       </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="57" t="s">
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="130" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="61">
+      <c r="I9" s="130"/>
+      <c r="J9" s="130"/>
+      <c r="K9" s="130"/>
+      <c r="L9" s="96">
         <f>EOMONTH($D$9,0)</f>
         <v>45107</v>
       </c>
-      <c r="M9" s="62"/>
-      <c r="N9" s="62"/>
-      <c r="O9" s="63"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="97"/>
+      <c r="O9" s="98"/>
     </row>
     <row r="10" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="64"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
+      <c r="A10" s="133"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="133"/>
+      <c r="N10" s="133"/>
+      <c r="O10" s="133"/>
     </row>
     <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="128" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="65"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="66"/>
-      <c r="K11" s="66"/>
-      <c r="L11" s="66"/>
-      <c r="M11" s="66"/>
-      <c r="N11" s="66"/>
-      <c r="O11" s="66"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="128"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="129"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
+      <c r="O11" s="129"/>
     </row>
     <row r="12" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="50"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="49" t="s">
+      <c r="B12" s="94"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="50"/>
-      <c r="G12" s="50"/>
-      <c r="H12" s="51"/>
-      <c r="I12" s="49" t="s">
+      <c r="F12" s="94"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="51"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="50"/>
-      <c r="O12" s="51"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="93"/>
+      <c r="L12" s="94"/>
+      <c r="M12" s="94"/>
+      <c r="N12" s="94"/>
+      <c r="O12" s="95"/>
     </row>
     <row r="13" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
+      <c r="A13" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="49" t="s">
+      <c r="B13" s="94"/>
+      <c r="C13" s="94"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="93" t="s">
         <v>61</v>
       </c>
-      <c r="F13" s="50"/>
-      <c r="G13" s="50"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="49" t="s">
+      <c r="F13" s="94"/>
+      <c r="G13" s="94"/>
+      <c r="H13" s="95"/>
+      <c r="I13" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="51"/>
-      <c r="K13" s="49" t="s">
+      <c r="J13" s="95"/>
+      <c r="K13" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="L13" s="50"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="50"/>
-      <c r="O13" s="51"/>
+      <c r="L13" s="94"/>
+      <c r="M13" s="94"/>
+      <c r="N13" s="94"/>
+      <c r="O13" s="95"/>
     </row>
     <row r="14" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
@@ -1851,1329 +1851,1329 @@
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
       <c r="D14" s="23"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="49" t="s">
+      <c r="E14" s="93"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="51"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="62"/>
-      <c r="M14" s="62"/>
-      <c r="N14" s="62"/>
-      <c r="O14" s="63"/>
+      <c r="J14" s="95"/>
+      <c r="K14" s="96"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="97"/>
+      <c r="O14" s="98"/>
     </row>
     <row r="15" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="67"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="67"/>
-      <c r="I15" s="67"/>
-      <c r="J15" s="67"/>
-      <c r="K15" s="67"/>
-      <c r="L15" s="67"/>
-      <c r="M15" s="67"/>
-      <c r="N15" s="67"/>
-      <c r="O15" s="67"/>
+      <c r="A15" s="99"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="99"/>
+      <c r="N15" s="99"/>
+      <c r="O15" s="99"/>
     </row>
     <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="55"/>
-      <c r="M16" s="55"/>
-      <c r="N16" s="55"/>
-      <c r="O16" s="56"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="101"/>
+      <c r="K16" s="101"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+      <c r="N16" s="101"/>
+      <c r="O16" s="102"/>
     </row>
     <row r="17" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="68"/>
-      <c r="C17" s="69" t="s">
+      <c r="A17" s="103" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="103"/>
+      <c r="C17" s="104" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="70"/>
-      <c r="E17" s="73" t="s">
+      <c r="D17" s="105"/>
+      <c r="E17" s="108" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="74"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="90" t="s">
+      <c r="F17" s="109"/>
+      <c r="G17" s="110"/>
+      <c r="H17" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="I17" s="91"/>
-      <c r="J17" s="91"/>
-      <c r="K17" s="91"/>
-      <c r="L17" s="91"/>
-      <c r="M17" s="91"/>
-      <c r="N17" s="91"/>
-      <c r="O17" s="92"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="126"/>
+      <c r="K17" s="126"/>
+      <c r="L17" s="126"/>
+      <c r="M17" s="126"/>
+      <c r="N17" s="126"/>
+      <c r="O17" s="127"/>
     </row>
     <row r="18" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="68"/>
-      <c r="B18" s="68"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="76" t="s">
+      <c r="A18" s="103"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="107"/>
+      <c r="E18" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="52"/>
-      <c r="G18" s="77"/>
-      <c r="H18" s="73" t="s">
+      <c r="F18" s="112"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="75"/>
-      <c r="J18" s="69" t="s">
+      <c r="I18" s="110"/>
+      <c r="J18" s="104" t="s">
         <v>17</v>
       </c>
-      <c r="K18" s="78"/>
-      <c r="L18" s="81" t="s">
+      <c r="K18" s="114"/>
+      <c r="L18" s="117" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="82"/>
-      <c r="N18" s="83" t="s">
+      <c r="M18" s="118"/>
+      <c r="N18" s="119" t="s">
         <v>19</v>
       </c>
-      <c r="O18" s="84"/>
+      <c r="O18" s="120"/>
     </row>
     <row r="19" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
-      <c r="B19" s="68"/>
-      <c r="C19" s="85" t="s">
+      <c r="A19" s="103"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="86"/>
-      <c r="E19" s="87" t="s">
+      <c r="D19" s="122"/>
+      <c r="E19" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="88"/>
-      <c r="G19" s="89"/>
+      <c r="F19" s="124"/>
+      <c r="G19" s="125"/>
       <c r="H19" s="24" t="s">
         <v>37</v>
       </c>
       <c r="I19" s="25"/>
-      <c r="J19" s="79"/>
-      <c r="K19" s="80"/>
-      <c r="L19" s="85" t="s">
+      <c r="J19" s="115"/>
+      <c r="K19" s="116"/>
+      <c r="L19" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="M19" s="86"/>
-      <c r="N19" s="87" t="s">
+      <c r="M19" s="122"/>
+      <c r="N19" s="123" t="s">
         <v>38</v>
       </c>
-      <c r="O19" s="89"/>
+      <c r="O19" s="125"/>
     </row>
     <row r="20" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="93">
+      <c r="A20" s="60">
         <f>IF(AND((ROW()-20)+EOMONTH($D$9,-1)+1&lt;=$L$9,(ROW()-20)+EOMONTH($D$9,-1)+1&gt;=$D$9),ROW()-19,"")</f>
         <v>1</v>
       </c>
-      <c r="B20" s="93"/>
-      <c r="C20" s="94">
+      <c r="B20" s="60"/>
+      <c r="C20" s="75">
         <f>IF($A20="","",IF($L20=0,1-J20-H20,0))</f>
         <v>1</v>
       </c>
-      <c r="D20" s="95"/>
-      <c r="E20" s="96">
+      <c r="D20" s="76"/>
+      <c r="E20" s="74">
         <f t="shared" ref="E20:E50" si="0">IF($A20="","",0)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="96"/>
-      <c r="G20" s="96"/>
-      <c r="H20" s="97">
+      <c r="F20" s="74"/>
+      <c r="G20" s="74"/>
+      <c r="H20" s="61">
         <f t="shared" ref="H20:H50" si="1">IF($A20="","",0)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="97"/>
-      <c r="J20" s="98">
+      <c r="I20" s="61"/>
+      <c r="J20" s="59">
         <f>IF($A20="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A20-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A20-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K20" s="98"/>
-      <c r="L20" s="96">
+      <c r="K20" s="59"/>
+      <c r="L20" s="74">
         <f>IF($A20="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A20-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A20-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M20" s="96"/>
-      <c r="N20" s="97">
+      <c r="M20" s="74"/>
+      <c r="N20" s="61">
         <f t="shared" ref="N20:N50" si="2">IF($A20="","",0)</f>
         <v>0</v>
       </c>
-      <c r="O20" s="97"/>
+      <c r="O20" s="61"/>
     </row>
     <row r="21" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="93">
+      <c r="A21" s="60">
         <f t="shared" ref="A21:A50" si="3">IF(AND((ROW()-20)+EOMONTH($D$9,-1)+1&lt;=$L$9,(ROW()-20)+EOMONTH($D$9,-1)+1&gt;=$D$9),ROW()-19,"")</f>
         <v>2</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="94">
+      <c r="B21" s="60"/>
+      <c r="C21" s="75">
         <f t="shared" ref="C21:C50" si="4">IF($A21="","",IF($L21=0,1-J21-H21,0))</f>
         <v>1</v>
       </c>
-      <c r="D21" s="95"/>
-      <c r="E21" s="96">
+      <c r="D21" s="76"/>
+      <c r="E21" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="96"/>
-      <c r="G21" s="96"/>
-      <c r="H21" s="97">
+      <c r="F21" s="74"/>
+      <c r="G21" s="74"/>
+      <c r="H21" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I21" s="97"/>
-      <c r="J21" s="98">
+      <c r="I21" s="61"/>
+      <c r="J21" s="59">
         <f>IF($A21="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A21-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A21-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K21" s="98"/>
-      <c r="L21" s="96">
+      <c r="K21" s="59"/>
+      <c r="L21" s="74">
         <f>IF($A21="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A21-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A21-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M21" s="96"/>
-      <c r="N21" s="97">
+      <c r="M21" s="74"/>
+      <c r="N21" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O21" s="97"/>
+      <c r="O21" s="61"/>
     </row>
     <row r="22" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="93">
+      <c r="A22" s="60">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="B22" s="93"/>
-      <c r="C22" s="94">
+      <c r="B22" s="60"/>
+      <c r="C22" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D22" s="95"/>
-      <c r="E22" s="96">
+      <c r="D22" s="76"/>
+      <c r="E22" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F22" s="96"/>
-      <c r="G22" s="96"/>
-      <c r="H22" s="97">
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I22" s="97"/>
-      <c r="J22" s="98">
+      <c r="I22" s="61"/>
+      <c r="J22" s="59">
         <f>IF($A22="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A22-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A22-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K22" s="98"/>
-      <c r="L22" s="96">
+      <c r="K22" s="59"/>
+      <c r="L22" s="74">
         <f>IF($A22="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A22-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A22-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M22" s="96"/>
-      <c r="N22" s="97">
+      <c r="M22" s="74"/>
+      <c r="N22" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O22" s="97"/>
+      <c r="O22" s="61"/>
     </row>
     <row r="23" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="93">
+      <c r="A23" s="60">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="94">
+      <c r="B23" s="60"/>
+      <c r="C23" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D23" s="95"/>
-      <c r="E23" s="96">
+      <c r="D23" s="76"/>
+      <c r="E23" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="97">
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I23" s="97"/>
-      <c r="J23" s="98">
+      <c r="I23" s="61"/>
+      <c r="J23" s="59">
         <f>IF($A23="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A23-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A23-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K23" s="98"/>
-      <c r="L23" s="96">
+      <c r="K23" s="59"/>
+      <c r="L23" s="74">
         <f>IF($A23="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A23-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A23-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M23" s="96"/>
-      <c r="N23" s="97">
+      <c r="M23" s="74"/>
+      <c r="N23" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O23" s="97"/>
+      <c r="O23" s="61"/>
     </row>
     <row r="24" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="93">
+      <c r="A24" s="60">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B24" s="93"/>
-      <c r="C24" s="94">
+      <c r="B24" s="60"/>
+      <c r="C24" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D24" s="95"/>
-      <c r="E24" s="96">
+      <c r="D24" s="76"/>
+      <c r="E24" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F24" s="96"/>
-      <c r="G24" s="96"/>
-      <c r="H24" s="97">
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I24" s="97"/>
-      <c r="J24" s="98">
+      <c r="I24" s="61"/>
+      <c r="J24" s="59">
         <f>IF($A24="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A24-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A24-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K24" s="98"/>
-      <c r="L24" s="96">
+      <c r="K24" s="59"/>
+      <c r="L24" s="74">
         <f>IF($A24="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A24-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A24-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M24" s="96"/>
-      <c r="N24" s="97">
+      <c r="M24" s="74"/>
+      <c r="N24" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O24" s="97"/>
+      <c r="O24" s="61"/>
     </row>
     <row r="25" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="93">
+      <c r="A25" s="60">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B25" s="93"/>
-      <c r="C25" s="94">
+      <c r="B25" s="60"/>
+      <c r="C25" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D25" s="95"/>
-      <c r="E25" s="96">
+      <c r="D25" s="76"/>
+      <c r="E25" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F25" s="96"/>
-      <c r="G25" s="96"/>
-      <c r="H25" s="97">
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I25" s="97"/>
-      <c r="J25" s="98">
+      <c r="I25" s="61"/>
+      <c r="J25" s="59">
         <f>IF($A25="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A25-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A25-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K25" s="98"/>
-      <c r="L25" s="96">
+      <c r="K25" s="59"/>
+      <c r="L25" s="74">
         <f>IF($A25="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A25-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A25-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M25" s="96"/>
-      <c r="N25" s="97">
+      <c r="M25" s="74"/>
+      <c r="N25" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O25" s="97"/>
+      <c r="O25" s="61"/>
     </row>
     <row r="26" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="93">
+      <c r="A26" s="60">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B26" s="93"/>
-      <c r="C26" s="94">
+      <c r="B26" s="60"/>
+      <c r="C26" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D26" s="95"/>
-      <c r="E26" s="96">
+      <c r="D26" s="76"/>
+      <c r="E26" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F26" s="96"/>
-      <c r="G26" s="96"/>
-      <c r="H26" s="97">
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I26" s="97"/>
-      <c r="J26" s="98">
+      <c r="I26" s="61"/>
+      <c r="J26" s="59">
         <f>IF($A26="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A26-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A26-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K26" s="98"/>
-      <c r="L26" s="96">
+      <c r="K26" s="59"/>
+      <c r="L26" s="74">
         <f>IF($A26="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A26-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A26-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M26" s="96"/>
-      <c r="N26" s="97">
+      <c r="M26" s="74"/>
+      <c r="N26" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O26" s="97"/>
+      <c r="O26" s="61"/>
     </row>
     <row r="27" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="93">
+      <c r="A27" s="60">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B27" s="93"/>
-      <c r="C27" s="94">
+      <c r="B27" s="60"/>
+      <c r="C27" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D27" s="95"/>
-      <c r="E27" s="96">
+      <c r="D27" s="76"/>
+      <c r="E27" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F27" s="96"/>
-      <c r="G27" s="96"/>
-      <c r="H27" s="97">
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I27" s="97"/>
-      <c r="J27" s="98">
+      <c r="I27" s="61"/>
+      <c r="J27" s="59">
         <f>IF($A27="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A27-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A27-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K27" s="98"/>
-      <c r="L27" s="96">
+      <c r="K27" s="59"/>
+      <c r="L27" s="74">
         <f>IF($A27="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A27-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A27-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M27" s="96"/>
-      <c r="N27" s="97">
+      <c r="M27" s="74"/>
+      <c r="N27" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O27" s="97"/>
+      <c r="O27" s="61"/>
     </row>
     <row r="28" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="93">
+      <c r="A28" s="60">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B28" s="93"/>
-      <c r="C28" s="94">
+      <c r="B28" s="60"/>
+      <c r="C28" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D28" s="95"/>
-      <c r="E28" s="96">
+      <c r="D28" s="76"/>
+      <c r="E28" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F28" s="96"/>
-      <c r="G28" s="96"/>
-      <c r="H28" s="97">
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I28" s="97"/>
-      <c r="J28" s="98">
+      <c r="I28" s="61"/>
+      <c r="J28" s="59">
         <f>IF($A28="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A28-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A28-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K28" s="98"/>
-      <c r="L28" s="96">
+      <c r="K28" s="59"/>
+      <c r="L28" s="74">
         <f>IF($A28="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A28-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A28-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M28" s="96"/>
-      <c r="N28" s="97">
+      <c r="M28" s="74"/>
+      <c r="N28" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O28" s="97"/>
+      <c r="O28" s="61"/>
     </row>
     <row r="29" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="93">
+      <c r="A29" s="60">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B29" s="93"/>
-      <c r="C29" s="94">
+      <c r="B29" s="60"/>
+      <c r="C29" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D29" s="95"/>
-      <c r="E29" s="96">
+      <c r="D29" s="76"/>
+      <c r="E29" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F29" s="96"/>
-      <c r="G29" s="96"/>
-      <c r="H29" s="97">
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I29" s="97"/>
-      <c r="J29" s="98">
+      <c r="I29" s="61"/>
+      <c r="J29" s="59">
         <f>IF($A29="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A29-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A29-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K29" s="98"/>
-      <c r="L29" s="96">
+      <c r="K29" s="59"/>
+      <c r="L29" s="74">
         <f>IF($A29="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A29-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A29-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M29" s="96"/>
-      <c r="N29" s="97">
+      <c r="M29" s="74"/>
+      <c r="N29" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O29" s="97"/>
+      <c r="O29" s="61"/>
     </row>
     <row r="30" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="93">
+      <c r="A30" s="60">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B30" s="93"/>
-      <c r="C30" s="94">
+      <c r="B30" s="60"/>
+      <c r="C30" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D30" s="95"/>
-      <c r="E30" s="96">
+      <c r="D30" s="76"/>
+      <c r="E30" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F30" s="96"/>
-      <c r="G30" s="96"/>
-      <c r="H30" s="97">
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I30" s="97"/>
-      <c r="J30" s="98">
+      <c r="I30" s="61"/>
+      <c r="J30" s="59">
         <f>IF($A30="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A30-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A30-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K30" s="98"/>
-      <c r="L30" s="96">
+      <c r="K30" s="59"/>
+      <c r="L30" s="74">
         <f>IF($A30="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A30-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A30-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M30" s="96"/>
-      <c r="N30" s="97">
+      <c r="M30" s="74"/>
+      <c r="N30" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O30" s="97"/>
+      <c r="O30" s="61"/>
     </row>
     <row r="31" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="93">
+      <c r="A31" s="60">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="B31" s="93"/>
-      <c r="C31" s="94">
+      <c r="B31" s="60"/>
+      <c r="C31" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D31" s="95"/>
-      <c r="E31" s="96">
+      <c r="D31" s="76"/>
+      <c r="E31" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F31" s="96"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="97">
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I31" s="97"/>
-      <c r="J31" s="98">
+      <c r="I31" s="61"/>
+      <c r="J31" s="59">
         <f>IF($A31="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A31-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A31-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K31" s="98"/>
-      <c r="L31" s="96">
+      <c r="K31" s="59"/>
+      <c r="L31" s="74">
         <f>IF($A31="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A31-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A31-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M31" s="96"/>
-      <c r="N31" s="97">
+      <c r="M31" s="74"/>
+      <c r="N31" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O31" s="97"/>
+      <c r="O31" s="61"/>
     </row>
     <row r="32" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="93">
+      <c r="A32" s="60">
         <f t="shared" si="3"/>
         <v>13</v>
       </c>
-      <c r="B32" s="93"/>
-      <c r="C32" s="94">
+      <c r="B32" s="60"/>
+      <c r="C32" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D32" s="95"/>
-      <c r="E32" s="96">
+      <c r="D32" s="76"/>
+      <c r="E32" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F32" s="96"/>
-      <c r="G32" s="96"/>
-      <c r="H32" s="97">
+      <c r="F32" s="74"/>
+      <c r="G32" s="74"/>
+      <c r="H32" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I32" s="97"/>
-      <c r="J32" s="98">
+      <c r="I32" s="61"/>
+      <c r="J32" s="59">
         <f>IF($A32="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A32-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A32-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K32" s="98"/>
-      <c r="L32" s="96">
+      <c r="K32" s="59"/>
+      <c r="L32" s="74">
         <f>IF($A32="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A32-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A32-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M32" s="96"/>
-      <c r="N32" s="97">
+      <c r="M32" s="74"/>
+      <c r="N32" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O32" s="97"/>
+      <c r="O32" s="61"/>
     </row>
     <row r="33" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="93">
+      <c r="A33" s="60">
         <f t="shared" si="3"/>
         <v>14</v>
       </c>
-      <c r="B33" s="93"/>
-      <c r="C33" s="94">
+      <c r="B33" s="60"/>
+      <c r="C33" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D33" s="95"/>
-      <c r="E33" s="96">
+      <c r="D33" s="76"/>
+      <c r="E33" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F33" s="96"/>
-      <c r="G33" s="96"/>
-      <c r="H33" s="97">
+      <c r="F33" s="74"/>
+      <c r="G33" s="74"/>
+      <c r="H33" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I33" s="97"/>
-      <c r="J33" s="98">
+      <c r="I33" s="61"/>
+      <c r="J33" s="59">
         <f>IF($A33="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A33-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A33-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K33" s="98"/>
-      <c r="L33" s="96">
+      <c r="K33" s="59"/>
+      <c r="L33" s="74">
         <f>IF($A33="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A33-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A33-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M33" s="96"/>
-      <c r="N33" s="97">
+      <c r="M33" s="74"/>
+      <c r="N33" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O33" s="97"/>
+      <c r="O33" s="61"/>
     </row>
     <row r="34" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="93">
+      <c r="A34" s="60">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="B34" s="93"/>
-      <c r="C34" s="94">
+      <c r="B34" s="60"/>
+      <c r="C34" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D34" s="95"/>
-      <c r="E34" s="96">
+      <c r="D34" s="76"/>
+      <c r="E34" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F34" s="96"/>
-      <c r="G34" s="96"/>
-      <c r="H34" s="97">
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I34" s="97"/>
-      <c r="J34" s="98">
+      <c r="I34" s="61"/>
+      <c r="J34" s="59">
         <f>IF($A34="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A34-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A34-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K34" s="98"/>
-      <c r="L34" s="96">
+      <c r="K34" s="59"/>
+      <c r="L34" s="74">
         <f>IF($A34="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A34-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A34-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M34" s="96"/>
-      <c r="N34" s="97">
+      <c r="M34" s="74"/>
+      <c r="N34" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O34" s="97"/>
+      <c r="O34" s="61"/>
     </row>
     <row r="35" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="93">
+      <c r="A35" s="60">
         <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B35" s="93"/>
-      <c r="C35" s="94">
+      <c r="B35" s="60"/>
+      <c r="C35" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D35" s="95"/>
-      <c r="E35" s="96">
+      <c r="D35" s="76"/>
+      <c r="E35" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F35" s="96"/>
-      <c r="G35" s="96"/>
-      <c r="H35" s="97">
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I35" s="97"/>
-      <c r="J35" s="98">
+      <c r="I35" s="61"/>
+      <c r="J35" s="59">
         <f>IF($A35="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A35-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A35-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K35" s="98"/>
-      <c r="L35" s="96">
+      <c r="K35" s="59"/>
+      <c r="L35" s="74">
         <f>IF($A35="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A35-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A35-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M35" s="96"/>
-      <c r="N35" s="97">
+      <c r="M35" s="74"/>
+      <c r="N35" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O35" s="97"/>
+      <c r="O35" s="61"/>
     </row>
     <row r="36" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="93">
+      <c r="A36" s="60">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
-      <c r="B36" s="93"/>
-      <c r="C36" s="94">
+      <c r="B36" s="60"/>
+      <c r="C36" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D36" s="95"/>
-      <c r="E36" s="96">
+      <c r="D36" s="76"/>
+      <c r="E36" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F36" s="96"/>
-      <c r="G36" s="96"/>
-      <c r="H36" s="97">
+      <c r="F36" s="74"/>
+      <c r="G36" s="74"/>
+      <c r="H36" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I36" s="97"/>
-      <c r="J36" s="98">
+      <c r="I36" s="61"/>
+      <c r="J36" s="59">
         <f>IF($A36="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A36-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A36-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K36" s="98"/>
-      <c r="L36" s="96">
+      <c r="K36" s="59"/>
+      <c r="L36" s="74">
         <f>IF($A36="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A36-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A36-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M36" s="96"/>
-      <c r="N36" s="97">
+      <c r="M36" s="74"/>
+      <c r="N36" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O36" s="97"/>
+      <c r="O36" s="61"/>
     </row>
     <row r="37" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="93">
+      <c r="A37" s="60">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="B37" s="93"/>
-      <c r="C37" s="94">
+      <c r="B37" s="60"/>
+      <c r="C37" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D37" s="95"/>
-      <c r="E37" s="96">
+      <c r="D37" s="76"/>
+      <c r="E37" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F37" s="96"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="97">
+      <c r="F37" s="74"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I37" s="97"/>
-      <c r="J37" s="98">
+      <c r="I37" s="61"/>
+      <c r="J37" s="59">
         <f>IF($A37="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A37-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A37-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K37" s="98"/>
-      <c r="L37" s="96">
+      <c r="K37" s="59"/>
+      <c r="L37" s="74">
         <f>IF($A37="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A37-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A37-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M37" s="96"/>
-      <c r="N37" s="97">
+      <c r="M37" s="74"/>
+      <c r="N37" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O37" s="97"/>
+      <c r="O37" s="61"/>
     </row>
     <row r="38" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="93">
+      <c r="A38" s="60">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
-      <c r="B38" s="93"/>
-      <c r="C38" s="94">
+      <c r="B38" s="60"/>
+      <c r="C38" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D38" s="95"/>
-      <c r="E38" s="96">
+      <c r="D38" s="76"/>
+      <c r="E38" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F38" s="96"/>
-      <c r="G38" s="96"/>
-      <c r="H38" s="97">
+      <c r="F38" s="74"/>
+      <c r="G38" s="74"/>
+      <c r="H38" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I38" s="97"/>
-      <c r="J38" s="98">
+      <c r="I38" s="61"/>
+      <c r="J38" s="59">
         <f>IF($A38="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A38-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A38-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K38" s="98"/>
-      <c r="L38" s="96">
+      <c r="K38" s="59"/>
+      <c r="L38" s="74">
         <f>IF($A38="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A38-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A38-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M38" s="96"/>
-      <c r="N38" s="97">
+      <c r="M38" s="74"/>
+      <c r="N38" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O38" s="97"/>
+      <c r="O38" s="61"/>
     </row>
     <row r="39" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="93">
+      <c r="A39" s="60">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
-      <c r="B39" s="93"/>
-      <c r="C39" s="94">
+      <c r="B39" s="60"/>
+      <c r="C39" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D39" s="95"/>
-      <c r="E39" s="96">
+      <c r="D39" s="76"/>
+      <c r="E39" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F39" s="96"/>
-      <c r="G39" s="96"/>
-      <c r="H39" s="97">
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I39" s="97"/>
-      <c r="J39" s="98">
+      <c r="I39" s="61"/>
+      <c r="J39" s="59">
         <f>IF($A39="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A39-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A39-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K39" s="98"/>
-      <c r="L39" s="96">
+      <c r="K39" s="59"/>
+      <c r="L39" s="74">
         <f>IF($A39="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A39-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A39-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M39" s="96"/>
-      <c r="N39" s="97">
+      <c r="M39" s="74"/>
+      <c r="N39" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O39" s="97"/>
+      <c r="O39" s="61"/>
     </row>
     <row r="40" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="93">
+      <c r="A40" s="60">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
-      <c r="B40" s="93"/>
-      <c r="C40" s="94">
+      <c r="B40" s="60"/>
+      <c r="C40" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D40" s="95"/>
-      <c r="E40" s="96">
+      <c r="D40" s="76"/>
+      <c r="E40" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F40" s="96"/>
-      <c r="G40" s="96"/>
-      <c r="H40" s="97">
+      <c r="F40" s="74"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I40" s="97"/>
-      <c r="J40" s="98">
+      <c r="I40" s="61"/>
+      <c r="J40" s="59">
         <f>IF($A40="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A40-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A40-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K40" s="98"/>
-      <c r="L40" s="96">
+      <c r="K40" s="59"/>
+      <c r="L40" s="74">
         <f>IF($A40="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A40-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A40-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M40" s="96"/>
-      <c r="N40" s="97">
+      <c r="M40" s="74"/>
+      <c r="N40" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O40" s="97"/>
+      <c r="O40" s="61"/>
     </row>
     <row r="41" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="93">
+      <c r="A41" s="60">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
-      <c r="B41" s="93"/>
-      <c r="C41" s="94">
+      <c r="B41" s="60"/>
+      <c r="C41" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D41" s="95"/>
-      <c r="E41" s="96">
+      <c r="D41" s="76"/>
+      <c r="E41" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F41" s="96"/>
-      <c r="G41" s="96"/>
-      <c r="H41" s="97">
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I41" s="97"/>
-      <c r="J41" s="98">
+      <c r="I41" s="61"/>
+      <c r="J41" s="59">
         <f>IF($A41="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A41-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A41-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K41" s="98"/>
-      <c r="L41" s="96">
+      <c r="K41" s="59"/>
+      <c r="L41" s="74">
         <f>IF($A41="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A41-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A41-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M41" s="96"/>
-      <c r="N41" s="97">
+      <c r="M41" s="74"/>
+      <c r="N41" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O41" s="97"/>
+      <c r="O41" s="61"/>
     </row>
     <row r="42" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="93">
+      <c r="A42" s="60">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
-      <c r="B42" s="93"/>
-      <c r="C42" s="94">
+      <c r="B42" s="60"/>
+      <c r="C42" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D42" s="95"/>
-      <c r="E42" s="96">
+      <c r="D42" s="76"/>
+      <c r="E42" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F42" s="96"/>
-      <c r="G42" s="96"/>
-      <c r="H42" s="97">
+      <c r="F42" s="74"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I42" s="97"/>
-      <c r="J42" s="98">
+      <c r="I42" s="61"/>
+      <c r="J42" s="59">
         <f>IF($A42="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A42-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A42-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K42" s="98"/>
-      <c r="L42" s="96">
+      <c r="K42" s="59"/>
+      <c r="L42" s="74">
         <f>IF($A42="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A42-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A42-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M42" s="96"/>
-      <c r="N42" s="97">
+      <c r="M42" s="74"/>
+      <c r="N42" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O42" s="97"/>
+      <c r="O42" s="61"/>
     </row>
     <row r="43" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="93">
+      <c r="A43" s="60">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
-      <c r="B43" s="93"/>
-      <c r="C43" s="94">
+      <c r="B43" s="60"/>
+      <c r="C43" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D43" s="95"/>
-      <c r="E43" s="96">
+      <c r="D43" s="76"/>
+      <c r="E43" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F43" s="96"/>
-      <c r="G43" s="96"/>
-      <c r="H43" s="97">
+      <c r="F43" s="74"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I43" s="97"/>
-      <c r="J43" s="98">
+      <c r="I43" s="61"/>
+      <c r="J43" s="59">
         <f>IF($A43="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A43-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A43-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K43" s="98"/>
-      <c r="L43" s="96">
+      <c r="K43" s="59"/>
+      <c r="L43" s="74">
         <f>IF($A43="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A43-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A43-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M43" s="96"/>
-      <c r="N43" s="97">
+      <c r="M43" s="74"/>
+      <c r="N43" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O43" s="97"/>
+      <c r="O43" s="61"/>
     </row>
     <row r="44" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="93">
+      <c r="A44" s="60">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
-      <c r="B44" s="93"/>
-      <c r="C44" s="94">
+      <c r="B44" s="60"/>
+      <c r="C44" s="75">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="D44" s="95"/>
-      <c r="E44" s="96">
+      <c r="D44" s="76"/>
+      <c r="E44" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F44" s="96"/>
-      <c r="G44" s="96"/>
-      <c r="H44" s="97">
+      <c r="F44" s="74"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I44" s="97"/>
-      <c r="J44" s="98">
+      <c r="I44" s="61"/>
+      <c r="J44" s="59">
         <f>IF($A44="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A44-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A44-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K44" s="98"/>
-      <c r="L44" s="96">
+      <c r="K44" s="59"/>
+      <c r="L44" s="74">
         <f>IF($A44="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A44-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A44-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>1</v>
       </c>
-      <c r="M44" s="96"/>
-      <c r="N44" s="97">
+      <c r="M44" s="74"/>
+      <c r="N44" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O44" s="97"/>
+      <c r="O44" s="61"/>
     </row>
     <row r="45" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="93">
+      <c r="A45" s="60">
         <f t="shared" si="3"/>
         <v>26</v>
       </c>
-      <c r="B45" s="93"/>
-      <c r="C45" s="94">
+      <c r="B45" s="60"/>
+      <c r="C45" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D45" s="95"/>
-      <c r="E45" s="96">
+      <c r="D45" s="76"/>
+      <c r="E45" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F45" s="96"/>
-      <c r="G45" s="96"/>
-      <c r="H45" s="97">
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I45" s="97"/>
-      <c r="J45" s="98">
+      <c r="I45" s="61"/>
+      <c r="J45" s="59">
         <f>IF($A45="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A45-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A45-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K45" s="98"/>
-      <c r="L45" s="96">
+      <c r="K45" s="59"/>
+      <c r="L45" s="74">
         <f>IF($A45="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A45-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A45-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M45" s="96"/>
-      <c r="N45" s="97">
+      <c r="M45" s="74"/>
+      <c r="N45" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O45" s="97"/>
+      <c r="O45" s="61"/>
     </row>
     <row r="46" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="93">
+      <c r="A46" s="60">
         <f t="shared" si="3"/>
         <v>27</v>
       </c>
-      <c r="B46" s="93"/>
-      <c r="C46" s="94">
+      <c r="B46" s="60"/>
+      <c r="C46" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D46" s="95"/>
-      <c r="E46" s="96">
+      <c r="D46" s="76"/>
+      <c r="E46" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F46" s="96"/>
-      <c r="G46" s="96"/>
-      <c r="H46" s="97">
+      <c r="F46" s="74"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I46" s="97"/>
-      <c r="J46" s="98">
+      <c r="I46" s="61"/>
+      <c r="J46" s="59">
         <f>IF($A46="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A46-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A46-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K46" s="98"/>
-      <c r="L46" s="96">
+      <c r="K46" s="59"/>
+      <c r="L46" s="74">
         <f>IF($A46="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A46-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A46-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M46" s="96"/>
-      <c r="N46" s="97">
+      <c r="M46" s="74"/>
+      <c r="N46" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O46" s="97"/>
+      <c r="O46" s="61"/>
     </row>
     <row r="47" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="93">
+      <c r="A47" s="60">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="94">
+      <c r="B47" s="60"/>
+      <c r="C47" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D47" s="95"/>
-      <c r="E47" s="96">
+      <c r="D47" s="76"/>
+      <c r="E47" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F47" s="96"/>
-      <c r="G47" s="96"/>
-      <c r="H47" s="97">
+      <c r="F47" s="74"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I47" s="97"/>
-      <c r="J47" s="98">
+      <c r="I47" s="61"/>
+      <c r="J47" s="59">
         <f>IF($A47="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A47-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A47-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K47" s="98"/>
-      <c r="L47" s="96">
+      <c r="K47" s="59"/>
+      <c r="L47" s="74">
         <f>IF($A47="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A47-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A47-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M47" s="96"/>
-      <c r="N47" s="97">
+      <c r="M47" s="74"/>
+      <c r="N47" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O47" s="97"/>
+      <c r="O47" s="61"/>
     </row>
     <row r="48" spans="1:15" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="93">
+      <c r="A48" s="60">
         <f t="shared" si="3"/>
         <v>29</v>
       </c>
-      <c r="B48" s="93"/>
-      <c r="C48" s="94">
+      <c r="B48" s="60"/>
+      <c r="C48" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D48" s="95"/>
-      <c r="E48" s="96">
+      <c r="D48" s="76"/>
+      <c r="E48" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F48" s="96"/>
-      <c r="G48" s="96"/>
-      <c r="H48" s="97">
+      <c r="F48" s="74"/>
+      <c r="G48" s="74"/>
+      <c r="H48" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I48" s="97"/>
-      <c r="J48" s="98">
+      <c r="I48" s="61"/>
+      <c r="J48" s="59">
         <f>IF($A48="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A48-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A48-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K48" s="98"/>
-      <c r="L48" s="96">
+      <c r="K48" s="59"/>
+      <c r="L48" s="74">
         <f>IF($A48="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A48-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A48-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M48" s="96"/>
-      <c r="N48" s="97">
+      <c r="M48" s="74"/>
+      <c r="N48" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O48" s="97"/>
+      <c r="O48" s="61"/>
     </row>
     <row r="49" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="93">
+      <c r="A49" s="60">
         <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="B49" s="93"/>
-      <c r="C49" s="94">
+      <c r="B49" s="60"/>
+      <c r="C49" s="75">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="D49" s="95"/>
-      <c r="E49" s="96">
+      <c r="D49" s="76"/>
+      <c r="E49" s="74">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F49" s="96"/>
-      <c r="G49" s="96"/>
-      <c r="H49" s="97">
+      <c r="F49" s="74"/>
+      <c r="G49" s="74"/>
+      <c r="H49" s="61">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I49" s="97"/>
-      <c r="J49" s="98">
+      <c r="I49" s="61"/>
+      <c r="J49" s="59">
         <f>IF($A49="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A49-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A49-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v>0</v>
       </c>
-      <c r="K49" s="98"/>
-      <c r="L49" s="96">
+      <c r="K49" s="59"/>
+      <c r="L49" s="74">
         <f>IF($A49="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A49-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A49-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v>0</v>
       </c>
-      <c r="M49" s="96"/>
-      <c r="N49" s="97">
+      <c r="M49" s="74"/>
+      <c r="N49" s="61">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O49" s="97"/>
+      <c r="O49" s="61"/>
     </row>
     <row r="50" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="93" t="str">
+      <c r="A50" s="60" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="B50" s="93"/>
-      <c r="C50" s="94" t="str">
+      <c r="B50" s="60"/>
+      <c r="C50" s="75" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="D50" s="95"/>
-      <c r="E50" s="96" t="str">
+      <c r="D50" s="76"/>
+      <c r="E50" s="74" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F50" s="96"/>
-      <c r="G50" s="96"/>
-      <c r="H50" s="97" t="str">
+      <c r="F50" s="74"/>
+      <c r="G50" s="74"/>
+      <c r="H50" s="61" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="I50" s="97"/>
-      <c r="J50" s="98" t="str">
+      <c r="I50" s="61"/>
+      <c r="J50" s="59" t="str">
         <f>IF($A50="","",IF(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A50-1,'Leave Days'!A:B,1,FALSE)),0,VLOOKUP(EOMONTH($D$9,-1)+1+$A50-1,'Leave Days'!A:B,2,FALSE)))</f>
         <v/>
       </c>
-      <c r="K50" s="98"/>
-      <c r="L50" s="96" t="str">
+      <c r="K50" s="59"/>
+      <c r="L50" s="74" t="str">
         <f>IF($A50="","",IF(AND(OR(WEEKDAY(EOMONTH($D$9,-1)+1+$A50-1,2)&gt;=6,NOT(ISNA(VLOOKUP(EOMONTH($D$9,-1)+1+$A50-1,'Public Holidays'!A:A,1,FALSE))))),1,0))</f>
         <v/>
       </c>
-      <c r="M50" s="96"/>
-      <c r="N50" s="97" t="str">
+      <c r="M50" s="74"/>
+      <c r="N50" s="61" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="O50" s="97"/>
+      <c r="O50" s="61"/>
     </row>
     <row r="51" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="26" t="s">
         <v>22</v>
       </c>
       <c r="B51" s="27"/>
-      <c r="C51" s="96">
+      <c r="C51" s="74">
         <f>SUM(C20:D50)</f>
         <v>21</v>
       </c>
-      <c r="D51" s="99"/>
-      <c r="E51" s="96">
+      <c r="D51" s="91"/>
+      <c r="E51" s="74">
         <f>SUM(E20:G50)</f>
         <v>0</v>
       </c>
-      <c r="F51" s="99"/>
-      <c r="G51" s="90"/>
+      <c r="F51" s="91"/>
+      <c r="G51" s="92"/>
       <c r="H51" s="7"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
@@ -3184,17 +3184,17 @@
       <c r="O51" s="9"/>
     </row>
     <row r="52" spans="1:15" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="124" t="s">
+      <c r="A52" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B52" s="125"/>
-      <c r="C52" s="125"/>
-      <c r="D52" s="126"/>
-      <c r="E52" s="130">
-        <v>0</v>
-      </c>
-      <c r="F52" s="131"/>
-      <c r="G52" s="132"/>
+      <c r="B52" s="80"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="85">
+        <v>0</v>
+      </c>
+      <c r="F52" s="86"/>
+      <c r="G52" s="87"/>
       <c r="H52" s="10"/>
       <c r="I52" s="11"/>
       <c r="J52" s="11"/>
@@ -3205,13 +3205,13 @@
       <c r="O52" s="12"/>
     </row>
     <row r="53" spans="1:15" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="127"/>
-      <c r="B53" s="128"/>
-      <c r="C53" s="128"/>
-      <c r="D53" s="129"/>
-      <c r="E53" s="133"/>
-      <c r="F53" s="134"/>
-      <c r="G53" s="135"/>
+      <c r="A53" s="82"/>
+      <c r="B53" s="83"/>
+      <c r="C53" s="83"/>
+      <c r="D53" s="84"/>
+      <c r="E53" s="88"/>
+      <c r="F53" s="89"/>
+      <c r="G53" s="90"/>
       <c r="H53" s="13"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
@@ -3248,34 +3248,34 @@
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="D55" s="17"/>
-      <c r="F55" s="108" t="s">
+      <c r="F55" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="G55" s="108"/>
-      <c r="H55" s="108"/>
-      <c r="I55" s="108"/>
-      <c r="J55" s="108"/>
-      <c r="K55" s="108"/>
-      <c r="L55" s="108"/>
-      <c r="M55" s="108"/>
-      <c r="N55" s="108"/>
-      <c r="O55" s="109"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="57"/>
+      <c r="I55" s="57"/>
+      <c r="J55" s="57"/>
+      <c r="K55" s="57"/>
+      <c r="L55" s="57"/>
+      <c r="M55" s="57"/>
+      <c r="N55" s="57"/>
+      <c r="O55" s="58"/>
     </row>
     <row r="56" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="37"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="D56" s="17"/>
-      <c r="F56" s="108"/>
-      <c r="G56" s="108"/>
-      <c r="H56" s="108"/>
-      <c r="I56" s="108"/>
-      <c r="J56" s="108"/>
-      <c r="K56" s="108"/>
-      <c r="L56" s="108"/>
-      <c r="M56" s="108"/>
-      <c r="N56" s="108"/>
-      <c r="O56" s="109"/>
+      <c r="F56" s="57"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="57"/>
+      <c r="J56" s="57"/>
+      <c r="K56" s="57"/>
+      <c r="L56" s="57"/>
+      <c r="M56" s="57"/>
+      <c r="N56" s="57"/>
+      <c r="O56" s="58"/>
     </row>
     <row r="57" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="33"/>
@@ -3296,31 +3296,31 @@
       <c r="O57" s="32"/>
     </row>
     <row r="58" spans="1:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="102" t="s">
+      <c r="A58" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="B58" s="103"/>
-      <c r="C58" s="103"/>
-      <c r="D58" s="104"/>
-      <c r="E58" s="113">
-        <v>0</v>
-      </c>
-      <c r="F58" s="113"/>
-      <c r="G58" s="113"/>
-      <c r="H58" s="113"/>
-      <c r="I58" s="113"/>
-      <c r="J58" s="113"/>
-      <c r="K58" s="113"/>
-      <c r="L58" s="113"/>
-      <c r="M58" s="113"/>
-      <c r="N58" s="113"/>
-      <c r="O58" s="114"/>
+      <c r="B58" s="52"/>
+      <c r="C58" s="52"/>
+      <c r="D58" s="53"/>
+      <c r="E58" s="65">
+        <v>0</v>
+      </c>
+      <c r="F58" s="65"/>
+      <c r="G58" s="65"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="65"/>
+      <c r="J58" s="65"/>
+      <c r="K58" s="65"/>
+      <c r="L58" s="65"/>
+      <c r="M58" s="65"/>
+      <c r="N58" s="65"/>
+      <c r="O58" s="66"/>
     </row>
     <row r="59" spans="1:15" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="105"/>
-      <c r="B59" s="106"/>
-      <c r="C59" s="106"/>
-      <c r="D59" s="107"/>
+      <c r="A59" s="54"/>
+      <c r="B59" s="55"/>
+      <c r="C59" s="55"/>
+      <c r="D59" s="56"/>
       <c r="E59" s="47"/>
       <c r="F59" s="47"/>
       <c r="G59" s="47"/>
@@ -3334,42 +3334,42 @@
       <c r="O59" s="48"/>
     </row>
     <row r="60" spans="1:15" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="115" t="s">
+      <c r="A60" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="116"/>
-      <c r="C60" s="116"/>
-      <c r="D60" s="117"/>
-      <c r="E60" s="118"/>
-      <c r="F60" s="119"/>
-      <c r="G60" s="119"/>
-      <c r="H60" s="119"/>
-      <c r="I60" s="119"/>
-      <c r="J60" s="119"/>
-      <c r="K60" s="119"/>
-      <c r="L60" s="119"/>
-      <c r="M60" s="119"/>
-      <c r="N60" s="119"/>
-      <c r="O60" s="120"/>
+      <c r="B60" s="68"/>
+      <c r="C60" s="68"/>
+      <c r="D60" s="69"/>
+      <c r="E60" s="70"/>
+      <c r="F60" s="71"/>
+      <c r="G60" s="71"/>
+      <c r="H60" s="71"/>
+      <c r="I60" s="71"/>
+      <c r="J60" s="71"/>
+      <c r="K60" s="71"/>
+      <c r="L60" s="71"/>
+      <c r="M60" s="71"/>
+      <c r="N60" s="71"/>
+      <c r="O60" s="72"/>
     </row>
     <row r="61" spans="1:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="121" t="s">
+      <c r="A61" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="B61" s="119"/>
-      <c r="C61" s="119"/>
-      <c r="D61" s="120"/>
-      <c r="E61" s="118"/>
-      <c r="F61" s="119"/>
-      <c r="G61" s="119"/>
-      <c r="H61" s="119"/>
-      <c r="I61" s="119"/>
-      <c r="J61" s="119"/>
-      <c r="K61" s="119"/>
-      <c r="L61" s="119"/>
-      <c r="M61" s="119"/>
-      <c r="N61" s="119"/>
-      <c r="O61" s="120"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="71"/>
+      <c r="D61" s="72"/>
+      <c r="E61" s="70"/>
+      <c r="F61" s="71"/>
+      <c r="G61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="I61" s="71"/>
+      <c r="J61" s="71"/>
+      <c r="K61" s="71"/>
+      <c r="L61" s="71"/>
+      <c r="M61" s="71"/>
+      <c r="N61" s="71"/>
+      <c r="O61" s="72"/>
     </row>
     <row r="62" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="18" t="s">
@@ -3396,56 +3396,56 @@
       <c r="A63" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B63" s="110" t="s">
+      <c r="B63" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C63" s="111"/>
-      <c r="D63" s="111"/>
-      <c r="E63" s="111"/>
-      <c r="F63" s="111"/>
-      <c r="G63" s="111"/>
-      <c r="H63" s="111"/>
-      <c r="I63" s="111"/>
-      <c r="J63" s="111"/>
-      <c r="K63" s="111"/>
-      <c r="L63" s="111"/>
-      <c r="M63" s="111"/>
-      <c r="N63" s="111"/>
-      <c r="O63" s="112"/>
+      <c r="C63" s="63"/>
+      <c r="D63" s="63"/>
+      <c r="E63" s="63"/>
+      <c r="F63" s="63"/>
+      <c r="G63" s="63"/>
+      <c r="H63" s="63"/>
+      <c r="I63" s="63"/>
+      <c r="J63" s="63"/>
+      <c r="K63" s="63"/>
+      <c r="L63" s="63"/>
+      <c r="M63" s="63"/>
+      <c r="N63" s="63"/>
+      <c r="O63" s="64"/>
     </row>
     <row r="64" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
-      <c r="B64" s="111"/>
-      <c r="C64" s="111"/>
-      <c r="D64" s="111"/>
-      <c r="E64" s="111"/>
-      <c r="F64" s="111"/>
-      <c r="G64" s="111"/>
-      <c r="H64" s="111"/>
-      <c r="I64" s="111"/>
-      <c r="J64" s="111"/>
-      <c r="K64" s="111"/>
-      <c r="L64" s="111"/>
-      <c r="M64" s="111"/>
-      <c r="N64" s="111"/>
-      <c r="O64" s="112"/>
+      <c r="B64" s="63"/>
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="63"/>
+      <c r="F64" s="63"/>
+      <c r="G64" s="63"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="63"/>
+      <c r="J64" s="63"/>
+      <c r="K64" s="63"/>
+      <c r="L64" s="63"/>
+      <c r="M64" s="63"/>
+      <c r="N64" s="63"/>
+      <c r="O64" s="64"/>
     </row>
     <row r="65" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20"/>
-      <c r="B65" s="111"/>
-      <c r="C65" s="111"/>
-      <c r="D65" s="111"/>
-      <c r="E65" s="111"/>
-      <c r="F65" s="111"/>
-      <c r="G65" s="111"/>
-      <c r="H65" s="111"/>
-      <c r="I65" s="111"/>
-      <c r="J65" s="111"/>
-      <c r="K65" s="111"/>
-      <c r="L65" s="111"/>
-      <c r="M65" s="111"/>
-      <c r="N65" s="111"/>
-      <c r="O65" s="112"/>
+      <c r="B65" s="63"/>
+      <c r="C65" s="63"/>
+      <c r="D65" s="63"/>
+      <c r="E65" s="63"/>
+      <c r="F65" s="63"/>
+      <c r="G65" s="63"/>
+      <c r="H65" s="63"/>
+      <c r="I65" s="63"/>
+      <c r="J65" s="63"/>
+      <c r="K65" s="63"/>
+      <c r="L65" s="63"/>
+      <c r="M65" s="63"/>
+      <c r="N65" s="63"/>
+      <c r="O65" s="64"/>
     </row>
     <row r="66" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
@@ -3472,56 +3472,56 @@
       <c r="A67" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B67" s="110" t="s">
+      <c r="B67" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="111"/>
-      <c r="D67" s="111"/>
-      <c r="E67" s="111"/>
-      <c r="F67" s="111"/>
-      <c r="G67" s="111"/>
-      <c r="H67" s="111"/>
-      <c r="I67" s="111"/>
-      <c r="J67" s="111"/>
-      <c r="K67" s="111"/>
-      <c r="L67" s="111"/>
-      <c r="M67" s="111"/>
-      <c r="N67" s="111"/>
-      <c r="O67" s="112"/>
+      <c r="C67" s="63"/>
+      <c r="D67" s="63"/>
+      <c r="E67" s="63"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="63"/>
+      <c r="H67" s="63"/>
+      <c r="I67" s="63"/>
+      <c r="J67" s="63"/>
+      <c r="K67" s="63"/>
+      <c r="L67" s="63"/>
+      <c r="M67" s="63"/>
+      <c r="N67" s="63"/>
+      <c r="O67" s="64"/>
     </row>
     <row r="68" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="111"/>
-      <c r="C68" s="111"/>
-      <c r="D68" s="111"/>
-      <c r="E68" s="111"/>
-      <c r="F68" s="111"/>
-      <c r="G68" s="111"/>
-      <c r="H68" s="111"/>
-      <c r="I68" s="111"/>
-      <c r="J68" s="111"/>
-      <c r="K68" s="111"/>
-      <c r="L68" s="111"/>
-      <c r="M68" s="111"/>
-      <c r="N68" s="111"/>
-      <c r="O68" s="112"/>
+      <c r="B68" s="63"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
+      <c r="G68" s="63"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="63"/>
+      <c r="J68" s="63"/>
+      <c r="K68" s="63"/>
+      <c r="L68" s="63"/>
+      <c r="M68" s="63"/>
+      <c r="N68" s="63"/>
+      <c r="O68" s="64"/>
     </row>
     <row r="69" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4"/>
-      <c r="B69" s="111"/>
-      <c r="C69" s="111"/>
-      <c r="D69" s="111"/>
-      <c r="E69" s="111"/>
-      <c r="F69" s="111"/>
-      <c r="G69" s="111"/>
-      <c r="H69" s="111"/>
-      <c r="I69" s="111"/>
-      <c r="J69" s="111"/>
-      <c r="K69" s="111"/>
-      <c r="L69" s="111"/>
-      <c r="M69" s="111"/>
-      <c r="N69" s="111"/>
-      <c r="O69" s="112"/>
+      <c r="B69" s="63"/>
+      <c r="C69" s="63"/>
+      <c r="D69" s="63"/>
+      <c r="E69" s="63"/>
+      <c r="F69" s="63"/>
+      <c r="G69" s="63"/>
+      <c r="H69" s="63"/>
+      <c r="I69" s="63"/>
+      <c r="J69" s="63"/>
+      <c r="K69" s="63"/>
+      <c r="L69" s="63"/>
+      <c r="M69" s="63"/>
+      <c r="N69" s="63"/>
+      <c r="O69" s="64"/>
     </row>
     <row r="70" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
@@ -3548,56 +3548,56 @@
       <c r="A71" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B71" s="122" t="s">
+      <c r="B71" s="77" t="s">
         <v>49</v>
       </c>
-      <c r="C71" s="122"/>
-      <c r="D71" s="122"/>
-      <c r="E71" s="122"/>
-      <c r="F71" s="122"/>
-      <c r="G71" s="122"/>
-      <c r="H71" s="122"/>
-      <c r="I71" s="122"/>
-      <c r="J71" s="122"/>
-      <c r="K71" s="122"/>
-      <c r="L71" s="122"/>
-      <c r="M71" s="122"/>
-      <c r="N71" s="122"/>
-      <c r="O71" s="123"/>
+      <c r="C71" s="77"/>
+      <c r="D71" s="77"/>
+      <c r="E71" s="77"/>
+      <c r="F71" s="77"/>
+      <c r="G71" s="77"/>
+      <c r="H71" s="77"/>
+      <c r="I71" s="77"/>
+      <c r="J71" s="77"/>
+      <c r="K71" s="77"/>
+      <c r="L71" s="77"/>
+      <c r="M71" s="77"/>
+      <c r="N71" s="77"/>
+      <c r="O71" s="78"/>
     </row>
     <row r="72" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4"/>
-      <c r="B72" s="122"/>
-      <c r="C72" s="122"/>
-      <c r="D72" s="122"/>
-      <c r="E72" s="122"/>
-      <c r="F72" s="122"/>
-      <c r="G72" s="122"/>
-      <c r="H72" s="122"/>
-      <c r="I72" s="122"/>
-      <c r="J72" s="122"/>
-      <c r="K72" s="122"/>
-      <c r="L72" s="122"/>
-      <c r="M72" s="122"/>
-      <c r="N72" s="122"/>
-      <c r="O72" s="123"/>
+      <c r="B72" s="77"/>
+      <c r="C72" s="77"/>
+      <c r="D72" s="77"/>
+      <c r="E72" s="77"/>
+      <c r="F72" s="77"/>
+      <c r="G72" s="77"/>
+      <c r="H72" s="77"/>
+      <c r="I72" s="77"/>
+      <c r="J72" s="77"/>
+      <c r="K72" s="77"/>
+      <c r="L72" s="77"/>
+      <c r="M72" s="77"/>
+      <c r="N72" s="77"/>
+      <c r="O72" s="78"/>
     </row>
     <row r="73" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="38"/>
-      <c r="B73" s="100"/>
-      <c r="C73" s="100"/>
-      <c r="D73" s="100"/>
-      <c r="E73" s="100"/>
-      <c r="F73" s="100"/>
-      <c r="G73" s="100"/>
-      <c r="H73" s="100"/>
-      <c r="I73" s="100"/>
-      <c r="J73" s="100"/>
-      <c r="K73" s="100"/>
-      <c r="L73" s="100"/>
-      <c r="M73" s="100"/>
-      <c r="N73" s="100"/>
-      <c r="O73" s="101"/>
+      <c r="B73" s="49"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="49"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="49"/>
+      <c r="G73" s="49"/>
+      <c r="H73" s="49"/>
+      <c r="I73" s="49"/>
+      <c r="J73" s="49"/>
+      <c r="K73" s="49"/>
+      <c r="L73" s="49"/>
+      <c r="M73" s="49"/>
+      <c r="N73" s="49"/>
+      <c r="O73" s="50"/>
     </row>
     <row r="75" spans="1:15" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="46" t="s">
@@ -3606,6 +3606,259 @@
     </row>
   </sheetData>
   <mergeCells count="277">
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:O7"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:O5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:O6"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="L8:O8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:K9"/>
+    <mergeCell ref="L9:O9"/>
+    <mergeCell ref="A10:O10"/>
+    <mergeCell ref="A11:O11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="K12:O12"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:O13"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="K14:O14"/>
+    <mergeCell ref="A15:O15"/>
+    <mergeCell ref="A16:O16"/>
+    <mergeCell ref="A17:B19"/>
+    <mergeCell ref="C17:D18"/>
+    <mergeCell ref="E17:G17"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K19"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="L19:M19"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="H17:O17"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="N20:O20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="L22:M22"/>
+    <mergeCell ref="N22:O22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="E24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="N24:O24"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="E23:G23"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="L25:M25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="L26:M26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="N28:O28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="L29:M29"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="E31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="N33:O33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="E32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="N35:O35"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="N34:O34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="L39:M39"/>
+    <mergeCell ref="N39:O39"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="L38:M38"/>
+    <mergeCell ref="N38:O38"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="E45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="J45:K45"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="N40:O40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="L41:M41"/>
+    <mergeCell ref="N41:O41"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="L40:M40"/>
+    <mergeCell ref="E40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L42:M42"/>
+    <mergeCell ref="N42:O42"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="E51:G51"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L47:M47"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="E50:G50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E49:G49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="E46:G46"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="J46:K46"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="J47:K47"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="E47:G47"/>
+    <mergeCell ref="H47:I47"/>
     <mergeCell ref="B73:O73"/>
     <mergeCell ref="A58:D59"/>
     <mergeCell ref="F55:O56"/>
@@ -3630,259 +3883,6 @@
     <mergeCell ref="N50:O50"/>
     <mergeCell ref="N48:O48"/>
     <mergeCell ref="N49:O49"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="E46:G46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="E47:G47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="E51:G51"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L47:M47"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="E50:G50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="E49:G49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L42:M42"/>
-    <mergeCell ref="N42:O42"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="N44:O44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="E45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="N40:O40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="L41:M41"/>
-    <mergeCell ref="N41:O41"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="L40:M40"/>
-    <mergeCell ref="E40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="N43:O43"/>
-    <mergeCell ref="L39:M39"/>
-    <mergeCell ref="N39:O39"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="L38:M38"/>
-    <mergeCell ref="N38:O38"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="L37:M37"/>
-    <mergeCell ref="N37:O37"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="E36:G36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="N34:O34"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="N33:O33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="E32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="L25:M25"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="E28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="N28:O28"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="E23:G23"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="N23:O23"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="L22:M22"/>
-    <mergeCell ref="N22:O22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="E24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="N24:O24"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="N20:O20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="K14:O14"/>
-    <mergeCell ref="A15:O15"/>
-    <mergeCell ref="A16:O16"/>
-    <mergeCell ref="A17:B19"/>
-    <mergeCell ref="C17:D18"/>
-    <mergeCell ref="E17:G17"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="J18:K19"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="N18:O18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="N19:O19"/>
-    <mergeCell ref="H17:O17"/>
-    <mergeCell ref="A11:O11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="K12:O12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="K13:O13"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:O8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:K9"/>
-    <mergeCell ref="L9:O9"/>
-    <mergeCell ref="A10:O10"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:O7"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:O5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:O6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A20:O50">
@@ -3905,27 +3905,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1026" r:id="rId4" name="CheckBox3">
+        <control shapeId="1030" r:id="rId4" name="CheckBox6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>53</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>56</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>53</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:colOff>219075</xdr:colOff>
+                <xdr:row>56</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1026" r:id="rId4" name="CheckBox3"/>
+        <control shapeId="1030" r:id="rId4" name="CheckBox6"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3955,27 +3955,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId8" name="CheckBox6">
+        <control shapeId="1026" r:id="rId8" name="CheckBox3">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
                 <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>56</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:row>53</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>4</xdr:col>
-                <xdr:colOff>219075</xdr:colOff>
-                <xdr:row>56</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>53</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1030" r:id="rId8" name="CheckBox6"/>
+        <control shapeId="1026" r:id="rId8" name="CheckBox3"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -4705,14 +4705,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="A4:C8"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.25" style="41" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" style="41" customWidth="1"/>
     <col min="2" max="2" width="17.125" style="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.625" style="41" customWidth="1"/>
   </cols>

</xml_diff>